<commit_message>
Schematic of LCD for manual
</commit_message>
<xml_diff>
--- a/To do list.xlsx
+++ b/To do list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Schematics</t>
   </si>
@@ -417,7 +417,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +542,9 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>